<commit_message>
Rubric Draft is added
</commit_message>
<xml_diff>
--- a/Weekly Reports/Metrics 22.10.2018.xlsx
+++ b/Weekly Reports/Metrics 22.10.2018.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC624E9E-0E54-4CC8-A09A-FEC248BEE004}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114D1571-CC1A-474D-952F-5F043B3B1578}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sayfa2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sayfa3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>Project 1</t>
   </si>
@@ -116,13 +118,46 @@
   </si>
   <si>
     <t>It can be funny,  there are some trends at industry in similarity with this projects.</t>
+  </si>
+  <si>
+    <t>Fast Execution</t>
+  </si>
+  <si>
+    <t>Robust</t>
+  </si>
+  <si>
+    <t>Low power</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Excellent </t>
+  </si>
+  <si>
+    <t>8 Good</t>
+  </si>
+  <si>
+    <t>6 Satisfactory</t>
+  </si>
+  <si>
+    <t>4 Avarage</t>
+  </si>
+  <si>
+    <t>2 Unacceptable</t>
+  </si>
+  <si>
+    <t>0 Unsatisfactory</t>
+  </si>
+  <si>
+    <t>Less</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,16 +165,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -258,11 +320,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -285,29 +358,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -496,6 +555,25 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -510,16 +588,15 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -535,17 +612,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{927FF8CB-3C9B-4815-B5CC-32EB78509356}" name="Tablo1" displayName="Tablo1" ref="A1:H5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{927FF8CB-3C9B-4815-B5CC-32EB78509356}" name="Tablo1" displayName="Tablo1" ref="A1:H5" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:H5" xr:uid="{51B643AD-84FD-415F-9F83-C76DCCFF3E61}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F1BEBFE4-F2E1-49E7-9428-FE50B1C81287}" name="Project\sMetrics" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{E48790AC-8480-49B6-8B33-DE3D49F2DA0A}" name="Image Processing Intensity" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{1D332500-920C-4C26-9602-CFBBA41AB3A0}" name="Mechanical Design  Challenges" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{D3610296-48AD-453F-9DF2-8E2F75FF026F}" name="Time Cost" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{399E420A-A402-4A48-9F5D-C65373F1E61C}" name="Manufacturability" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{63A71ED8-6A91-4443-83C5-02AC2559DC68}" name="Amount of Subsystem" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{2409C5FA-70E8-4A60-806E-E45C38E45D0F}" name="Know-How" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{7DF07D73-E134-4571-94FE-2F8AB77E138B}" name="Fun" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{F1BEBFE4-F2E1-49E7-9428-FE50B1C81287}" name="Project\sMetrics" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{E48790AC-8480-49B6-8B33-DE3D49F2DA0A}" name="Image Processing Intensity" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{1D332500-920C-4C26-9602-CFBBA41AB3A0}" name="Mechanical Design  Challenges" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{D3610296-48AD-453F-9DF2-8E2F75FF026F}" name="Time Cost" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{399E420A-A402-4A48-9F5D-C65373F1E61C}" name="Manufacturability" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{63A71ED8-6A91-4443-83C5-02AC2559DC68}" name="Amount of Subsystem" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{2409C5FA-70E8-4A60-806E-E45C38E45D0F}" name="Know-How" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{7DF07D73-E134-4571-94FE-2F8AB77E138B}" name="Fun" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -816,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,4 +1046,290 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7CF828-7560-4D00-AD8F-B12F240E4FF7}">
+  <dimension ref="B1:J33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="11">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <f>B2+C2+D2+E2+F2+G2+H2+I2</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="13">
+        <f>B2/59</f>
+        <v>0.10169491525423729</v>
+      </c>
+      <c r="C3" s="13">
+        <f t="shared" ref="C3:I3" si="0">C2/59</f>
+        <v>8.4745762711864403E-2</v>
+      </c>
+      <c r="D3" s="13">
+        <f t="shared" si="0"/>
+        <v>0.15254237288135594</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" si="0"/>
+        <v>0.16949152542372881</v>
+      </c>
+      <c r="F3" s="13">
+        <f t="shared" si="0"/>
+        <v>0.16949152542372881</v>
+      </c>
+      <c r="G3" s="13">
+        <f t="shared" si="0"/>
+        <v>0.10169491525423729</v>
+      </c>
+      <c r="H3" s="13">
+        <f>H2/59</f>
+        <v>0.13559322033898305</v>
+      </c>
+      <c r="I3" s="13">
+        <f t="shared" si="0"/>
+        <v>8.4745762711864403E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0.08</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.17</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.18</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D14" s="13">
+        <v>0.08</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0.17</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0.18</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5F7E54-6652-4CB1-B5E0-9D3F32986EE3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Metrics of the projects are created, and the projects are weighted.
</commit_message>
<xml_diff>
--- a/Weekly Reports/Metrics 22.10.2018.xlsx
+++ b/Weekly Reports/Metrics 22.10.2018.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114D1571-CC1A-474D-952F-5F043B3B1578}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089D713D-6DB6-4331-BBD2-33D972F74024}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,17 +12,22 @@
     <sheet name="Sayfa2" sheetId="2" r:id="rId2"/>
     <sheet name="Sayfa3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Project 1</t>
   </si>
@@ -120,44 +125,104 @@
     <t>It can be funny,  there are some trends at industry in similarity with this projects.</t>
   </si>
   <si>
-    <t>Fast Execution</t>
-  </si>
-  <si>
     <t>Robust</t>
   </si>
   <si>
-    <t>Low power</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
-    <t xml:space="preserve">10 Excellent </t>
-  </si>
-  <si>
-    <t>8 Good</t>
-  </si>
-  <si>
-    <t>6 Satisfactory</t>
-  </si>
-  <si>
-    <t>4 Avarage</t>
-  </si>
-  <si>
-    <t>2 Unacceptable</t>
-  </si>
-  <si>
     <t>0 Unsatisfactory</t>
   </si>
   <si>
-    <t>Less</t>
+    <t>Minimum work load is required.</t>
+  </si>
+  <si>
+    <t>No work load is required.</t>
+  </si>
+  <si>
+    <t>The project totally depends on image processing.</t>
+  </si>
+  <si>
+    <t>Image processing is intensive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Excellent </t>
+  </si>
+  <si>
+    <t>2 Good</t>
+  </si>
+  <si>
+    <t>1 Unacceptable</t>
+  </si>
+  <si>
+    <t>Less is better.</t>
+  </si>
+  <si>
+    <t>Mechanical arms and joints are required.</t>
+  </si>
+  <si>
+    <t>Junction and suspension system is requierd.</t>
+  </si>
+  <si>
+    <t>Procurement of materials is effortless.</t>
+  </si>
+  <si>
+    <t>Unique materials are required, such as 3D printers and CNC machinary.</t>
+  </si>
+  <si>
+    <t>Totally stranger.</t>
+  </si>
+  <si>
+    <t>Familiar.</t>
+  </si>
+  <si>
+    <t>Knowledge.</t>
+  </si>
+  <si>
+    <t>Joyless.</t>
+  </si>
+  <si>
+    <t>Some phases of the project is funny.</t>
+  </si>
+  <si>
+    <t>Project 1 Weighted</t>
+  </si>
+  <si>
+    <t>Project 2 Weighted</t>
+  </si>
+  <si>
+    <t>Project 3 Weighted</t>
+  </si>
+  <si>
+    <t>Project 4 Weighted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> All team members have fun during the project.</t>
+  </si>
+  <si>
+    <t>No operation failure wrt environmental changes.</t>
+  </si>
+  <si>
+    <t>Can be optimised to changing environmental conditions.</t>
+  </si>
+  <si>
+    <t>Can sufficiently work in the specified environment.</t>
+  </si>
+  <si>
+    <t>Some modules can be hand-crafted</t>
+  </si>
+  <si>
+    <t>A module is needed to re-invented.</t>
+  </si>
+  <si>
+    <t>Project mainly depends on paperwork.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,15 +238,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,12 +249,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor theme="4"/>
       </patternFill>
     </fill>
@@ -335,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -359,9 +411,20 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,6 +663,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFDC57B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1050,23 +1118,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7CF828-7560-4D00-AD8F-B12F240E4FF7}">
-  <dimension ref="B1:J33"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="10" t="s">
         <v>5</v>
       </c>
@@ -1082,240 +1151,372 @@
       <c r="F1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="12" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="B2" s="12">
+        <v>0.13</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="E2" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F2" s="12">
+        <v>0.21</v>
+      </c>
+      <c r="G2" s="12">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7">
+        <f>B3*B2</f>
+        <v>0.13</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:G7" si="0">C3*C2</f>
+        <v>0.11</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.42</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.51</v>
+      </c>
+      <c r="H7">
+        <f>G7+F7+E7+D7+C7+B7</f>
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8">
+        <f>B4*B2</f>
+        <v>0.26</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:G8" si="1">C4*C2</f>
+        <v>0.22</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0.36</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.34</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ref="H8:H10" si="2">G8+F8+E8+D8+C8+B8</f>
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9">
+        <f>B2*B5</f>
+        <v>0.26</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:G9" si="3">C2*C5</f>
+        <v>0.22</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="3"/>
+        <v>0.54</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>0.63</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>0.34</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>2.3900000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10">
+        <f>B2*B6</f>
+        <v>0.39</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:G10" si="4">C2*C6</f>
+        <v>0.22</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="4"/>
+        <v>0.36</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="4"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>0.63</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>0.51</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>2.7100000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="11">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <v>8</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <f>B2+C2+D2+E2+F2+G2+H2+I2</f>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="13">
-        <f>B2/59</f>
-        <v>0.10169491525423729</v>
-      </c>
-      <c r="C3" s="13">
-        <f t="shared" ref="C3:I3" si="0">C2/59</f>
-        <v>8.4745762711864403E-2</v>
-      </c>
-      <c r="D3" s="13">
-        <f t="shared" si="0"/>
-        <v>0.15254237288135594</v>
-      </c>
-      <c r="E3" s="13">
-        <f t="shared" si="0"/>
-        <v>0.16949152542372881</v>
-      </c>
-      <c r="F3" s="13">
-        <f t="shared" si="0"/>
-        <v>0.16949152542372881</v>
-      </c>
-      <c r="G3" s="13">
-        <f t="shared" si="0"/>
-        <v>0.10169491525423729</v>
-      </c>
-      <c r="H3" s="13">
-        <f>H2/59</f>
-        <v>0.13559322033898305</v>
-      </c>
-      <c r="I3" s="13">
-        <f t="shared" si="0"/>
-        <v>8.4745762711864403E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="C7" s="13">
-        <v>0.08</v>
-      </c>
-      <c r="D7" s="13">
-        <v>0.15</v>
-      </c>
-      <c r="E7" s="13">
-        <v>0.17</v>
-      </c>
-      <c r="F7" s="13">
-        <v>0.18</v>
-      </c>
-      <c r="G7" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="H7" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I7" s="13">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D14" s="13">
-        <v>0.08</v>
-      </c>
-      <c r="E14" s="13">
-        <v>0.15</v>
-      </c>
-      <c r="F14" s="13">
-        <v>0.17</v>
-      </c>
-      <c r="G14" s="13">
-        <v>0.18</v>
-      </c>
-      <c r="H14" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="I14" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J14" s="13">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="13">
+        <f ca="1">+E18+C16:G19+B13:G19+A13:G19+E18+C16:G19</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C27" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>41</v>
-      </c>
-    </row>
+    <row r="28" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Metrics are updated, it is more straight forward
</commit_message>
<xml_diff>
--- a/Weekly Reports/Metrics 22.10.2018.xlsx
+++ b/Weekly Reports/Metrics 22.10.2018.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089D713D-6DB6-4331-BBD2-33D972F74024}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589EB57E-86E2-4C0E-BD54-796A65419617}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,22 +12,17 @@
     <sheet name="Sayfa2" sheetId="2" r:id="rId2"/>
     <sheet name="Sayfa3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
   <si>
     <t>Project 1</t>
   </si>
@@ -134,18 +129,9 @@
     <t>0 Unsatisfactory</t>
   </si>
   <si>
-    <t>Minimum work load is required.</t>
-  </si>
-  <si>
-    <t>No work load is required.</t>
-  </si>
-  <si>
     <t>The project totally depends on image processing.</t>
   </si>
   <si>
-    <t>Image processing is intensive.</t>
-  </si>
-  <si>
     <t xml:space="preserve">3 Excellent </t>
   </si>
   <si>
@@ -155,36 +141,21 @@
     <t>1 Unacceptable</t>
   </si>
   <si>
-    <t>Less is better.</t>
-  </si>
-  <si>
     <t>Mechanical arms and joints are required.</t>
   </si>
   <si>
     <t>Junction and suspension system is requierd.</t>
   </si>
   <si>
-    <t>Procurement of materials is effortless.</t>
-  </si>
-  <si>
     <t>Unique materials are required, such as 3D printers and CNC machinary.</t>
   </si>
   <si>
     <t>Totally stranger.</t>
   </si>
   <si>
-    <t>Familiar.</t>
-  </si>
-  <si>
-    <t>Knowledge.</t>
-  </si>
-  <si>
     <t>Joyless.</t>
   </si>
   <si>
-    <t>Some phases of the project is funny.</t>
-  </si>
-  <si>
     <t>Project 1 Weighted</t>
   </si>
   <si>
@@ -200,22 +171,55 @@
     <t xml:space="preserve"> All team members have fun during the project.</t>
   </si>
   <si>
-    <t>No operation failure wrt environmental changes.</t>
-  </si>
-  <si>
-    <t>Can be optimised to changing environmental conditions.</t>
-  </si>
-  <si>
-    <t>Can sufficiently work in the specified environment.</t>
-  </si>
-  <si>
-    <t>Some modules can be hand-crafted</t>
-  </si>
-  <si>
     <t>A module is needed to re-invented.</t>
   </si>
   <si>
-    <t>Project mainly depends on paperwork.</t>
+    <t>Project can be made without image processing.</t>
+  </si>
+  <si>
+    <t>Iımage process is assistant to make the project.</t>
+  </si>
+  <si>
+    <t>The project is based on image processing.</t>
+  </si>
+  <si>
+    <t>No calculations and therotical information about mechanical design is not required.</t>
+  </si>
+  <si>
+    <t>Some basic mechanical components such as junction can be used.</t>
+  </si>
+  <si>
+    <t>Procurement of materials is effortless, no need special components that are created at 3D printer and CNC.</t>
+  </si>
+  <si>
+    <t>Some modules can be hand-crafted.</t>
+  </si>
+  <si>
+    <t>In past, we worked on the similar project.</t>
+  </si>
+  <si>
+    <t>We are aware of the concepts basis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only, we heard the concept. </t>
+  </si>
+  <si>
+    <t>Three of team members have fun during the project.</t>
+  </si>
+  <si>
+    <t>Two or less of team members have fun during the project.</t>
+  </si>
+  <si>
+    <t>No operation failure with respect to environmental changes.</t>
+  </si>
+  <si>
+    <t>The project only works at specific condition.</t>
+  </si>
+  <si>
+    <t>The projects can not work properly with respect to condition.</t>
+  </si>
+  <si>
+    <t>The project can be optimized for working at different conditions.</t>
   </si>
 </sst>
 </file>
@@ -239,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,8 +256,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -369,17 +379,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -411,20 +410,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1120,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7CF828-7560-4D00-AD8F-B12F240E4FF7}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,6 +1133,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="12"/>
       <c r="B1" s="10" t="s">
         <v>5</v>
       </c>
@@ -1151,366 +1149,368 @@
       <c r="F1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="15">
         <v>0.13</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="15">
         <v>0.11</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="15">
         <v>0.18</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="15">
         <v>0.2</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="15">
         <v>0.21</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="15">
         <v>0.17</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="12">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="12">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="12">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="12">
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="12">
         <v>2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="12">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="12">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="12">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="12">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="12">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="12">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="12">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="12">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="12">
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="12">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="12">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="12">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="12">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="12">
         <v>2</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="12">
         <v>3</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="12">
         <v>3</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="12">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="12">
         <f>B3*B2</f>
         <v>0.13</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="12">
         <f t="shared" ref="C7:G7" si="0">C3*C2</f>
         <v>0.11</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="12">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="12">
         <f t="shared" si="0"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="12">
         <f t="shared" si="0"/>
         <v>0.42</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="12">
         <f t="shared" si="0"/>
         <v>0.51</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="12">
         <f>G7+F7+E7+D7+C7+B7</f>
         <v>2.13</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="12">
         <f>B4*B2</f>
         <v>0.26</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="12">
         <f t="shared" ref="C8:G8" si="1">C4*C2</f>
         <v>0.22</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="12">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="12">
         <f t="shared" si="1"/>
         <v>0.34</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="12">
         <f t="shared" ref="H8:H10" si="2">G8+F8+E8+D8+C8+B8</f>
         <v>1.18</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="12">
         <f>B2*B5</f>
         <v>0.26</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="12">
         <f t="shared" ref="C9:G9" si="3">C2*C5</f>
         <v>0.22</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="12">
         <f t="shared" si="3"/>
         <v>0.54</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="12">
         <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="12">
         <f t="shared" si="3"/>
         <v>0.63</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="12">
         <f t="shared" si="3"/>
         <v>0.34</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="12">
         <f t="shared" si="2"/>
         <v>2.3900000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="12">
         <f>B2*B6</f>
         <v>0.39</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="12">
         <f t="shared" ref="C10:G10" si="4">C2*C6</f>
         <v>0.22</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="12">
         <f t="shared" si="4"/>
         <v>0.36</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="12">
         <f t="shared" si="4"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="12">
         <f t="shared" si="4"/>
         <v>0.63</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="12">
         <f t="shared" si="4"/>
         <v>0.51</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="12">
         <f t="shared" si="2"/>
         <v>2.7100000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="13" t="s">
+      <c r="D19" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="E19" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="13" t="s">
+      <c r="F19" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="13">
-        <f ca="1">+E18+C16:G19+B13:G19+A13:G19+E18+C16:G19</f>
-        <v>0</v>
+      <c r="G19" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update style of metrics
</commit_message>
<xml_diff>
--- a/Weekly Reports/Metrics 22.10.2018.xlsx
+++ b/Weekly Reports/Metrics 22.10.2018.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589EB57E-86E2-4C0E-BD54-796A65419617}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1215B6F-0E27-4D18-9BC1-7C823BA93BC4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="66">
   <si>
     <t>Project 1</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Joyless.</t>
   </si>
   <si>
-    <t>Project 1 Weighted</t>
-  </si>
-  <si>
     <t>Project 2 Weighted</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>The project can be optimized for working at different conditions.</t>
+  </si>
+  <si>
+    <t>Project 1  Weighted</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -422,6 +422,12 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1118,16 +1124,16 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.140625" customWidth="1"/>
     <col min="7" max="7" width="26.85546875" customWidth="1"/>
   </cols>
@@ -1153,7 +1159,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>33</v>
       </c>
@@ -1176,7 +1182,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
@@ -1222,7 +1228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
@@ -1245,7 +1251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
@@ -1268,134 +1274,134 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="12">
+    <row r="7" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="18">
         <f>B3*B2</f>
         <v>0.13</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="18">
         <f t="shared" ref="C7:G7" si="0">C3*C2</f>
         <v>0.11</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="18">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="18">
         <f t="shared" si="0"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="18">
         <f t="shared" si="0"/>
         <v>0.42</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="18">
         <f t="shared" si="0"/>
         <v>0.51</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="18">
         <f>G7+F7+E7+D7+C7+B7</f>
         <v>2.13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="12">
+    <row r="8" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="18">
         <f>B4*B2</f>
         <v>0.26</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="18">
         <f t="shared" ref="C8:G8" si="1">C4*C2</f>
         <v>0.22</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="18">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="18">
         <f t="shared" si="1"/>
         <v>0.34</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="18">
         <f t="shared" ref="H8:H10" si="2">G8+F8+E8+D8+C8+B8</f>
         <v>1.18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="12">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="18">
         <f>B2*B5</f>
         <v>0.26</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="18">
         <f t="shared" ref="C9:G9" si="3">C2*C5</f>
         <v>0.22</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="18">
         <f t="shared" si="3"/>
         <v>0.54</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="18">
         <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="18">
         <f t="shared" si="3"/>
         <v>0.63</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="18">
         <f t="shared" si="3"/>
         <v>0.34</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="18">
         <f t="shared" si="2"/>
         <v>2.3900000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="12">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="18">
         <f>B2*B6</f>
         <v>0.39</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="18">
         <f t="shared" ref="C10:G10" si="4">C2*C6</f>
         <v>0.22</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="18">
         <f t="shared" si="4"/>
         <v>0.36</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="18">
         <f t="shared" si="4"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="18">
         <f t="shared" si="4"/>
         <v>0.63</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="18">
         <f t="shared" si="4"/>
         <v>0.51</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="18">
         <f t="shared" si="2"/>
         <v>2.7100000000000004</v>
       </c>
@@ -1426,22 +1432,22 @@
         <v>36</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1449,22 +1455,22 @@
         <v>37</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1472,7 +1478,7 @@
         <v>38</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>40</v>
@@ -1481,13 +1487,13 @@
         <v>41</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1501,7 +1507,7 @@
         <v>39</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>42</v>
@@ -1510,10 +1516,125 @@
         <v>43</v>
       </c>
       <c r="G19" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D28" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="29" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Metices are slightly corrected and coloured.
</commit_message>
<xml_diff>
--- a/Weekly Reports/Metrics 22.10.2018.xlsx
+++ b/Weekly Reports/Metrics 22.10.2018.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1215B6F-0E27-4D18-9BC1-7C823BA93BC4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B5335E-78C8-4B0D-B603-F2668950C248}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,17 +12,22 @@
     <sheet name="Sayfa2" sheetId="2" r:id="rId2"/>
     <sheet name="Sayfa3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="68">
   <si>
     <t>Project 1</t>
   </si>
@@ -153,9 +158,6 @@
     <t>Totally stranger.</t>
   </si>
   <si>
-    <t>Joyless.</t>
-  </si>
-  <si>
     <t>Project 2 Weighted</t>
   </si>
   <si>
@@ -165,9 +167,6 @@
     <t>Project 4 Weighted</t>
   </si>
   <si>
-    <t xml:space="preserve"> All team members have fun during the project.</t>
-  </si>
-  <si>
     <t>A module is needed to re-invented.</t>
   </si>
   <si>
@@ -201,25 +200,37 @@
     <t xml:space="preserve">Only, we heard the concept. </t>
   </si>
   <si>
-    <t>Three of team members have fun during the project.</t>
-  </si>
-  <si>
     <t>Two or less of team members have fun during the project.</t>
   </si>
   <si>
     <t>No operation failure with respect to environmental changes.</t>
   </si>
   <si>
-    <t>The project only works at specific condition.</t>
-  </si>
-  <si>
-    <t>The projects can not work properly with respect to condition.</t>
-  </si>
-  <si>
     <t>The project can be optimized for working at different conditions.</t>
   </si>
   <si>
     <t>Project 1  Weighted</t>
+  </si>
+  <si>
+    <t>The project only works at the specified condition.</t>
+  </si>
+  <si>
+    <t>The projects can not work properly with respect to the specified condition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> All team members can have fun during the project.</t>
+  </si>
+  <si>
+    <t>Three of team members can have fun during the project.</t>
+  </si>
+  <si>
+    <t>Two or less of team members can have fun during the project.</t>
+  </si>
+  <si>
+    <t>None of team members can have fun during the project.</t>
+  </si>
+  <si>
+    <t>None of team members can have fun during the project..</t>
   </si>
 </sst>
 </file>
@@ -243,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +273,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -386,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -409,24 +456,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1123,23 +1199,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7CF828-7560-4D00-AD8F-B12F240E4FF7}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1"/>
+    <col min="1" max="16384" width="30" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="12"/>
+      <c r="A1" s="11"/>
       <c r="B1" s="10" t="s">
         <v>5</v>
       </c>
@@ -1160,479 +1230,479 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>0.13</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="14">
         <v>0.11</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>0.18</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>0.2</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>0.21</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="14">
         <v>0.17</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="24">
         <v>1</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="24">
         <v>1</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="23">
         <v>2</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="22">
         <v>3</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="23">
         <v>2</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="22">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="23">
         <v>2</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="23">
         <v>2</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="23">
         <v>2</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>0</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>0</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="23">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="23">
         <v>2</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="23">
         <v>2</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="22">
         <v>3</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="23">
         <v>2</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="22">
         <v>3</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="23">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="22">
         <v>3</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="23">
         <v>2</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="23">
         <v>2</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="22">
         <v>3</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="22">
         <v>3</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="18">
+    <row r="7" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="11">
         <f>B3*B2</f>
         <v>0.13</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="25">
         <f t="shared" ref="C7:G7" si="0">C3*C2</f>
         <v>0.11</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="23">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="22">
         <f t="shared" si="0"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="23">
         <f t="shared" si="0"/>
         <v>0.42</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="22">
         <f t="shared" si="0"/>
         <v>0.51</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="11">
         <f>G7+F7+E7+D7+C7+B7</f>
         <v>2.13</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="18">
+      <c r="A8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="23">
         <f>B4*B2</f>
         <v>0.26</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="23">
         <f t="shared" ref="C8:G8" si="1">C4*C2</f>
         <v>0.22</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="23">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="23">
         <f t="shared" si="1"/>
         <v>0.34</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="11">
         <f t="shared" ref="H8:H10" si="2">G8+F8+E8+D8+C8+B8</f>
         <v>1.18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="18">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="23">
         <f>B2*B5</f>
         <v>0.26</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="23">
         <f t="shared" ref="C9:G9" si="3">C2*C5</f>
         <v>0.22</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="22">
         <f t="shared" si="3"/>
         <v>0.54</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="23">
         <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="22">
         <f t="shared" si="3"/>
         <v>0.63</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="23">
         <f t="shared" si="3"/>
         <v>0.34</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="11">
         <f t="shared" si="2"/>
         <v>2.3900000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="18">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="22">
         <f>B2*B6</f>
         <v>0.39</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="23">
         <f t="shared" ref="C10:G10" si="4">C2*C6</f>
         <v>0.22</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="23">
         <f t="shared" si="4"/>
         <v>0.36</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="22">
         <f t="shared" si="4"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="22">
         <f t="shared" si="4"/>
         <v>0.63</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="22">
         <f t="shared" si="4"/>
         <v>0.51</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="13">
         <f t="shared" si="2"/>
         <v>2.7100000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="11" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C18" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="C25" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="C26" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="14" t="s">
+      <c r="E26" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="14" t="s">
+      <c r="E28" s="19" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>